<commit_message>
esta funcional en ON and Day and Night
</commit_message>
<xml_diff>
--- a/PlanStaff.xlsx
+++ b/PlanStaff.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operations_best_opt" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -72,21 +72,8 @@
       <family val="2"/>
       <sz val="11"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <color indexed="81"/>
-      <sz val="9"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color indexed="81"/>
-      <sz val="9"/>
-    </font>
   </fonts>
-  <fills count="45">
+  <fills count="47">
     <fill>
       <patternFill/>
     </fill>
@@ -347,8 +334,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00C6EFCE"/>
         <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF99"/>
+        <bgColor rgb="00FFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -717,24 +716,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="46" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="46" fontId="5" fillId="40" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,9 +770,23 @@
     <xf numFmtId="46" fontId="5" fillId="43" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,10 +1265,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AWU15"/>
+  <dimension ref="A1:AWU14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:ASW11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -19222,7 +19217,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="OP4" s="79" t="inlineStr">
+      <c r="OP4" s="108" t="inlineStr">
         <is>
           <t>On call NS</t>
         </is>
@@ -19602,7 +19597,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="RN4" s="79" t="inlineStr">
+      <c r="RN4" s="108" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
@@ -20467,7 +20462,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="YE4" s="79" t="n"/>
+      <c r="YE4" s="108" t="n"/>
       <c r="YF4" s="10" t="inlineStr">
         <is>
           <t>On</t>
@@ -20568,7 +20563,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="YZ4" s="79" t="inlineStr">
+      <c r="YZ4" s="108" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
@@ -21093,7 +21088,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ADA4" s="79" t="inlineStr">
+      <c r="ADA4" s="108" t="inlineStr">
         <is>
           <t>Transition</t>
         </is>
@@ -21513,7 +21508,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AGG4" s="79" t="inlineStr">
+      <c r="AGG4" s="108" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
@@ -21593,7 +21588,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AGW4" s="79" t="inlineStr">
+      <c r="AGW4" s="108" t="inlineStr">
         <is>
           <t>change</t>
         </is>
@@ -22073,7 +22068,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AKO4" s="82" t="inlineStr">
+      <c r="AKO4" s="109" t="inlineStr">
         <is>
           <t>On call NS</t>
         </is>
@@ -26321,7 +26316,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="XJ5" s="79" t="n"/>
+      <c r="XJ5" s="108" t="n"/>
       <c r="XK5" s="10" t="inlineStr">
         <is>
           <t>Night</t>
@@ -26947,7 +26942,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ACF5" s="80" t="n"/>
+      <c r="ACF5" s="107" t="n"/>
       <c r="ACG5" s="10" t="inlineStr">
         <is>
           <t>On</t>
@@ -28098,7 +28093,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="ALC5" s="82" t="inlineStr">
+      <c r="ALC5" s="109" t="inlineStr">
         <is>
           <t>On call NS</t>
         </is>
@@ -35724,7 +35719,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="FZ7" s="82" t="n"/>
+      <c r="FZ7" s="109" t="n"/>
       <c r="GA7" s="10" t="inlineStr">
         <is>
           <t>Day</t>
@@ -37709,15 +37704,15 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="XG7" s="79" t="inlineStr">
+      <c r="XG7" s="108" t="inlineStr">
         <is>
           <t>BAITALI FUEL TRUCK</t>
         </is>
       </c>
-      <c r="XH7" s="109" t="n"/>
-      <c r="XI7" s="109" t="n"/>
-      <c r="XJ7" s="109" t="n"/>
-      <c r="XK7" s="110" t="n"/>
+      <c r="XH7" s="105" t="n"/>
+      <c r="XI7" s="105" t="n"/>
+      <c r="XJ7" s="105" t="n"/>
+      <c r="XK7" s="106" t="n"/>
       <c r="XL7" s="11" t="inlineStr">
         <is>
           <t>Off</t>
@@ -37728,15 +37723,15 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="XN7" s="82" t="inlineStr">
+      <c r="XN7" s="109" t="inlineStr">
         <is>
           <t>BAITALI FUEL TRUCK and Waiting docs for HR induction</t>
         </is>
       </c>
-      <c r="XO7" s="109" t="n"/>
-      <c r="XP7" s="109" t="n"/>
-      <c r="XQ7" s="109" t="n"/>
-      <c r="XR7" s="110" t="n"/>
+      <c r="XO7" s="105" t="n"/>
+      <c r="XP7" s="105" t="n"/>
+      <c r="XQ7" s="105" t="n"/>
+      <c r="XR7" s="106" t="n"/>
       <c r="XS7" s="11" t="inlineStr">
         <is>
           <t>Off</t>
@@ -37747,71 +37742,71 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="XU7" s="80" t="inlineStr">
+      <c r="XU7" s="107" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="XV7" s="109" t="n"/>
-      <c r="XW7" s="109" t="n"/>
-      <c r="XX7" s="109" t="n"/>
-      <c r="XY7" s="110" t="n"/>
-      <c r="XZ7" s="80" t="inlineStr">
+      <c r="XV7" s="105" t="n"/>
+      <c r="XW7" s="105" t="n"/>
+      <c r="XX7" s="105" t="n"/>
+      <c r="XY7" s="106" t="n"/>
+      <c r="XZ7" s="107" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YA7" s="109" t="n"/>
-      <c r="YB7" s="109" t="n"/>
-      <c r="YC7" s="109" t="n"/>
-      <c r="YD7" s="110" t="n"/>
-      <c r="YE7" s="80" t="inlineStr">
+      <c r="YA7" s="105" t="n"/>
+      <c r="YB7" s="105" t="n"/>
+      <c r="YC7" s="105" t="n"/>
+      <c r="YD7" s="106" t="n"/>
+      <c r="YE7" s="107" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YF7" s="109" t="n"/>
-      <c r="YG7" s="109" t="n"/>
-      <c r="YH7" s="109" t="n"/>
-      <c r="YI7" s="110" t="n"/>
-      <c r="YJ7" s="80" t="inlineStr">
+      <c r="YF7" s="105" t="n"/>
+      <c r="YG7" s="105" t="n"/>
+      <c r="YH7" s="105" t="n"/>
+      <c r="YI7" s="106" t="n"/>
+      <c r="YJ7" s="107" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YK7" s="109" t="n"/>
-      <c r="YL7" s="109" t="n"/>
-      <c r="YM7" s="109" t="n"/>
-      <c r="YN7" s="110" t="n"/>
-      <c r="YO7" s="81" t="inlineStr">
+      <c r="YK7" s="105" t="n"/>
+      <c r="YL7" s="105" t="n"/>
+      <c r="YM7" s="105" t="n"/>
+      <c r="YN7" s="106" t="n"/>
+      <c r="YO7" s="104" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YP7" s="109" t="n"/>
-      <c r="YQ7" s="109" t="n"/>
-      <c r="YR7" s="109" t="n"/>
-      <c r="YS7" s="110" t="n"/>
-      <c r="YT7" s="81" t="inlineStr">
+      <c r="YP7" s="105" t="n"/>
+      <c r="YQ7" s="105" t="n"/>
+      <c r="YR7" s="105" t="n"/>
+      <c r="YS7" s="106" t="n"/>
+      <c r="YT7" s="104" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YU7" s="109" t="n"/>
-      <c r="YV7" s="109" t="n"/>
-      <c r="YW7" s="109" t="n"/>
-      <c r="YX7" s="110" t="n"/>
-      <c r="YY7" s="81" t="inlineStr">
+      <c r="YU7" s="105" t="n"/>
+      <c r="YV7" s="105" t="n"/>
+      <c r="YW7" s="105" t="n"/>
+      <c r="YX7" s="106" t="n"/>
+      <c r="YY7" s="104" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YZ7" s="109" t="n"/>
-      <c r="ZA7" s="109" t="n"/>
-      <c r="ZB7" s="109" t="n"/>
-      <c r="ZC7" s="109" t="n"/>
-      <c r="ZD7" s="110" t="n"/>
-      <c r="ZE7" s="81" t="inlineStr">
+      <c r="YZ7" s="105" t="n"/>
+      <c r="ZA7" s="105" t="n"/>
+      <c r="ZB7" s="105" t="n"/>
+      <c r="ZC7" s="105" t="n"/>
+      <c r="ZD7" s="106" t="n"/>
+      <c r="ZE7" s="104" t="inlineStr">
         <is>
           <t>RGM HR</t>
         </is>
@@ -38251,7 +38246,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ACO7" s="79" t="n"/>
+      <c r="ACO7" s="108" t="n"/>
       <c r="ACP7" s="10" t="inlineStr">
         <is>
           <t>On</t>
@@ -43005,7 +43000,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="TH8" s="79" t="n"/>
+      <c r="TH8" s="108" t="n"/>
       <c r="TI8" s="10" t="inlineStr">
         <is>
           <t>Day</t>
@@ -48553,7 +48548,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="QC9" s="79" t="n"/>
+      <c r="QC9" s="108" t="n"/>
       <c r="QD9" s="10" t="inlineStr">
         <is>
           <t>Day</t>
@@ -50334,7 +50329,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ADV9" s="79" t="inlineStr">
+      <c r="ADV9" s="108" t="inlineStr">
         <is>
           <t>Transitio</t>
         </is>
@@ -51144,7 +51139,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AKB9" s="79" t="inlineStr">
+      <c r="AKB9" s="108" t="inlineStr">
         <is>
           <t>On call</t>
         </is>
@@ -52257,13 +52252,13 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="ASX9" s="79" t="n"/>
-      <c r="ASY9" s="79" t="n"/>
-      <c r="ASZ9" s="79" t="n"/>
-      <c r="ATA9" s="79" t="n"/>
-      <c r="ATB9" s="79" t="n"/>
-      <c r="ATC9" s="79" t="n"/>
-      <c r="ATD9" s="79" t="n"/>
+      <c r="ASX9" s="108" t="n"/>
+      <c r="ASY9" s="108" t="n"/>
+      <c r="ASZ9" s="108" t="n"/>
+      <c r="ATA9" s="108" t="n"/>
+      <c r="ATB9" s="108" t="n"/>
+      <c r="ATC9" s="108" t="n"/>
+      <c r="ATD9" s="108" t="n"/>
     </row>
     <row r="10" ht="30" customFormat="1" customHeight="1" s="8">
       <c r="A10" s="77" t="inlineStr">
@@ -53045,7 +53040,7 @@
       <c r="ACK10" s="29" t="n"/>
       <c r="ACL10" s="29" t="n"/>
       <c r="ACM10" s="31" t="n"/>
-      <c r="ACN10" s="82" t="n"/>
+      <c r="ACN10" s="109" t="n"/>
       <c r="ACO10" s="31" t="n"/>
       <c r="ACP10" s="31" t="n"/>
       <c r="ACQ10" s="31" t="n"/>
@@ -53168,15 +53163,15 @@
       <c r="AHD10" s="45" t="n"/>
       <c r="AHE10" s="45" t="n"/>
       <c r="AHF10" s="45" t="n"/>
-      <c r="AHG10" s="82" t="n"/>
-      <c r="AHH10" s="82" t="n"/>
-      <c r="AHI10" s="82" t="n"/>
-      <c r="AHJ10" s="82" t="n"/>
-      <c r="AHK10" s="82" t="n"/>
-      <c r="AHL10" s="82" t="n"/>
-      <c r="AHM10" s="82" t="n"/>
-      <c r="AHN10" s="82" t="n"/>
-      <c r="AHO10" s="82" t="n"/>
+      <c r="AHG10" s="109" t="n"/>
+      <c r="AHH10" s="109" t="n"/>
+      <c r="AHI10" s="109" t="n"/>
+      <c r="AHJ10" s="109" t="n"/>
+      <c r="AHK10" s="109" t="n"/>
+      <c r="AHL10" s="109" t="n"/>
+      <c r="AHM10" s="109" t="n"/>
+      <c r="AHN10" s="109" t="n"/>
+      <c r="AHO10" s="109" t="n"/>
       <c r="AHP10" s="42" t="n"/>
       <c r="AHQ10" s="42" t="n"/>
       <c r="AHR10" s="42" t="n"/>
@@ -53230,27 +53225,27 @@
       <c r="AJN10" s="42" t="n"/>
       <c r="AJO10" s="42" t="n"/>
       <c r="AJP10" s="42" t="n"/>
-      <c r="AJQ10" s="79" t="inlineStr">
+      <c r="AJQ10" s="108" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJR10" s="79" t="inlineStr">
+      <c r="AJR10" s="108" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJS10" s="79" t="inlineStr">
+      <c r="AJS10" s="108" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJT10" s="79" t="inlineStr">
+      <c r="AJT10" s="108" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJU10" s="79" t="inlineStr">
+      <c r="AJU10" s="108" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
@@ -53265,7 +53260,7 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="AJX10" s="79" t="inlineStr">
+      <c r="AJX10" s="108" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
@@ -54956,83 +54951,83 @@
       <c r="TT11" s="42" t="n"/>
       <c r="TU11" s="42" t="n"/>
       <c r="TV11" s="42" t="n"/>
-      <c r="TW11" s="82" t="n"/>
-      <c r="TX11" s="82" t="n"/>
+      <c r="TW11" s="109" t="n"/>
+      <c r="TX11" s="109" t="n"/>
       <c r="TY11" s="11" t="n"/>
       <c r="TZ11" s="11" t="n"/>
-      <c r="UA11" s="82" t="n"/>
-      <c r="UB11" s="82" t="n"/>
-      <c r="UC11" s="82" t="n"/>
-      <c r="UD11" s="82" t="n"/>
-      <c r="UE11" s="82" t="n"/>
-      <c r="UF11" s="82" t="n"/>
-      <c r="UG11" s="82" t="n"/>
-      <c r="UH11" s="82" t="n"/>
-      <c r="UI11" s="82" t="n"/>
-      <c r="UJ11" s="82" t="n"/>
+      <c r="UA11" s="109" t="n"/>
+      <c r="UB11" s="109" t="n"/>
+      <c r="UC11" s="109" t="n"/>
+      <c r="UD11" s="109" t="n"/>
+      <c r="UE11" s="109" t="n"/>
+      <c r="UF11" s="109" t="n"/>
+      <c r="UG11" s="109" t="n"/>
+      <c r="UH11" s="109" t="n"/>
+      <c r="UI11" s="109" t="n"/>
+      <c r="UJ11" s="109" t="n"/>
       <c r="UK11" s="31" t="n"/>
       <c r="UL11" s="31" t="n"/>
       <c r="UM11" s="31" t="n"/>
       <c r="UN11" s="31" t="n"/>
-      <c r="UO11" s="92" t="n"/>
-      <c r="UP11" s="92" t="n"/>
-      <c r="UQ11" s="92" t="n"/>
-      <c r="UR11" s="92" t="n"/>
-      <c r="US11" s="92" t="n"/>
-      <c r="UT11" s="92" t="n"/>
-      <c r="UU11" s="92" t="n"/>
-      <c r="UV11" s="92" t="n"/>
-      <c r="UW11" s="92" t="n"/>
-      <c r="UX11" s="92" t="n"/>
-      <c r="UY11" s="92" t="n"/>
-      <c r="UZ11" s="92" t="n"/>
-      <c r="VA11" s="92" t="n"/>
-      <c r="VB11" s="92" t="n"/>
-      <c r="VC11" s="92" t="n"/>
-      <c r="VD11" s="92" t="n"/>
-      <c r="VE11" s="92" t="n"/>
-      <c r="VF11" s="92" t="n"/>
-      <c r="VG11" s="92" t="n"/>
-      <c r="VH11" s="92" t="n"/>
-      <c r="VI11" s="92" t="n"/>
-      <c r="VJ11" s="92" t="n"/>
-      <c r="VK11" s="92" t="n"/>
-      <c r="VL11" s="92" t="n"/>
-      <c r="VM11" s="92" t="n"/>
-      <c r="VN11" s="92" t="n"/>
-      <c r="VO11" s="92" t="n"/>
-      <c r="VP11" s="92" t="n"/>
-      <c r="VQ11" s="92" t="n"/>
-      <c r="VR11" s="92" t="n"/>
-      <c r="VS11" s="92" t="n"/>
-      <c r="VT11" s="92" t="n"/>
-      <c r="VU11" s="92" t="n"/>
-      <c r="VV11" s="92" t="n"/>
-      <c r="VW11" s="92" t="n"/>
-      <c r="VX11" s="92" t="n"/>
-      <c r="VY11" s="92" t="n"/>
-      <c r="VZ11" s="92" t="n"/>
-      <c r="WA11" s="92" t="n"/>
-      <c r="WB11" s="92" t="n"/>
-      <c r="WC11" s="92" t="n"/>
-      <c r="WD11" s="92" t="n"/>
-      <c r="WE11" s="92" t="n"/>
-      <c r="WF11" s="92" t="n"/>
-      <c r="WG11" s="92" t="n"/>
-      <c r="WH11" s="92" t="n"/>
-      <c r="WI11" s="92" t="n"/>
-      <c r="WJ11" s="92" t="n"/>
-      <c r="WK11" s="92" t="n"/>
-      <c r="WL11" s="92" t="n"/>
-      <c r="WM11" s="92" t="n"/>
-      <c r="WN11" s="92" t="n"/>
-      <c r="WO11" s="92" t="n"/>
-      <c r="WP11" s="92" t="n"/>
-      <c r="WQ11" s="92" t="n"/>
-      <c r="WR11" s="92" t="n"/>
-      <c r="WS11" s="92" t="n"/>
-      <c r="WT11" s="92" t="n"/>
-      <c r="WU11" s="92" t="n"/>
+      <c r="UO11" s="86" t="n"/>
+      <c r="UP11" s="86" t="n"/>
+      <c r="UQ11" s="86" t="n"/>
+      <c r="UR11" s="86" t="n"/>
+      <c r="US11" s="86" t="n"/>
+      <c r="UT11" s="86" t="n"/>
+      <c r="UU11" s="86" t="n"/>
+      <c r="UV11" s="86" t="n"/>
+      <c r="UW11" s="86" t="n"/>
+      <c r="UX11" s="86" t="n"/>
+      <c r="UY11" s="86" t="n"/>
+      <c r="UZ11" s="86" t="n"/>
+      <c r="VA11" s="86" t="n"/>
+      <c r="VB11" s="86" t="n"/>
+      <c r="VC11" s="86" t="n"/>
+      <c r="VD11" s="86" t="n"/>
+      <c r="VE11" s="86" t="n"/>
+      <c r="VF11" s="86" t="n"/>
+      <c r="VG11" s="86" t="n"/>
+      <c r="VH11" s="86" t="n"/>
+      <c r="VI11" s="86" t="n"/>
+      <c r="VJ11" s="86" t="n"/>
+      <c r="VK11" s="86" t="n"/>
+      <c r="VL11" s="86" t="n"/>
+      <c r="VM11" s="86" t="n"/>
+      <c r="VN11" s="86" t="n"/>
+      <c r="VO11" s="86" t="n"/>
+      <c r="VP11" s="86" t="n"/>
+      <c r="VQ11" s="86" t="n"/>
+      <c r="VR11" s="86" t="n"/>
+      <c r="VS11" s="86" t="n"/>
+      <c r="VT11" s="86" t="n"/>
+      <c r="VU11" s="86" t="n"/>
+      <c r="VV11" s="86" t="n"/>
+      <c r="VW11" s="86" t="n"/>
+      <c r="VX11" s="86" t="n"/>
+      <c r="VY11" s="86" t="n"/>
+      <c r="VZ11" s="86" t="n"/>
+      <c r="WA11" s="86" t="n"/>
+      <c r="WB11" s="86" t="n"/>
+      <c r="WC11" s="86" t="n"/>
+      <c r="WD11" s="86" t="n"/>
+      <c r="WE11" s="86" t="n"/>
+      <c r="WF11" s="86" t="n"/>
+      <c r="WG11" s="86" t="n"/>
+      <c r="WH11" s="86" t="n"/>
+      <c r="WI11" s="86" t="n"/>
+      <c r="WJ11" s="86" t="n"/>
+      <c r="WK11" s="86" t="n"/>
+      <c r="WL11" s="86" t="n"/>
+      <c r="WM11" s="86" t="n"/>
+      <c r="WN11" s="86" t="n"/>
+      <c r="WO11" s="86" t="n"/>
+      <c r="WP11" s="86" t="n"/>
+      <c r="WQ11" s="86" t="n"/>
+      <c r="WR11" s="86" t="n"/>
+      <c r="WS11" s="86" t="n"/>
+      <c r="WT11" s="86" t="n"/>
+      <c r="WU11" s="86" t="n"/>
       <c r="WV11" s="42" t="n"/>
       <c r="WW11" s="42" t="n"/>
       <c r="WX11" s="42" t="n"/>
@@ -55059,143 +55054,143 @@
       <c r="XS11" s="42" t="n"/>
       <c r="XT11" s="42" t="n"/>
       <c r="XU11" s="42" t="n"/>
-      <c r="XV11" s="82" t="n"/>
-      <c r="XW11" s="82" t="n"/>
-      <c r="XX11" s="82" t="n"/>
-      <c r="XY11" s="80" t="n"/>
-      <c r="XZ11" s="80" t="n"/>
-      <c r="YA11" s="80" t="n"/>
-      <c r="YB11" s="80" t="n"/>
-      <c r="YC11" s="80" t="n"/>
-      <c r="YD11" s="80" t="n"/>
-      <c r="YE11" s="80" t="n"/>
-      <c r="YF11" s="80" t="n"/>
-      <c r="YG11" s="80" t="n"/>
-      <c r="YH11" s="80" t="n"/>
-      <c r="YI11" s="80" t="n"/>
-      <c r="YJ11" s="80" t="n"/>
-      <c r="YK11" s="80" t="n"/>
-      <c r="YL11" s="80" t="n"/>
-      <c r="YM11" s="93" t="n"/>
-      <c r="YN11" s="93" t="n"/>
-      <c r="YO11" s="93" t="n"/>
-      <c r="YP11" s="93" t="n"/>
-      <c r="YQ11" s="93" t="n"/>
-      <c r="YR11" s="93" t="n"/>
-      <c r="YS11" s="93" t="n"/>
-      <c r="YT11" s="93" t="n"/>
-      <c r="YU11" s="93" t="n"/>
-      <c r="YV11" s="93" t="n"/>
-      <c r="YW11" s="93" t="n"/>
-      <c r="YX11" s="93" t="n"/>
-      <c r="YY11" s="93" t="n"/>
-      <c r="YZ11" s="93" t="n"/>
-      <c r="ZA11" s="93" t="n"/>
-      <c r="ZB11" s="93" t="n"/>
-      <c r="ZC11" s="93" t="n"/>
-      <c r="ZD11" s="93" t="n"/>
-      <c r="ZE11" s="93" t="n"/>
-      <c r="ZF11" s="93" t="n"/>
-      <c r="ZG11" s="93" t="n"/>
-      <c r="ZH11" s="94" t="n"/>
-      <c r="ZI11" s="94" t="n"/>
-      <c r="ZJ11" s="94" t="n"/>
-      <c r="ZK11" s="94" t="n"/>
-      <c r="ZL11" s="94" t="n"/>
-      <c r="ZM11" s="94" t="n"/>
-      <c r="ZN11" s="94" t="n"/>
-      <c r="ZO11" s="94" t="n"/>
-      <c r="ZP11" s="94" t="n"/>
-      <c r="ZQ11" s="94" t="n"/>
-      <c r="ZR11" s="94" t="n"/>
-      <c r="ZS11" s="94" t="n"/>
-      <c r="ZT11" s="94" t="n"/>
-      <c r="ZU11" s="94" t="n"/>
-      <c r="ZV11" s="94" t="n"/>
-      <c r="ZW11" s="94" t="n"/>
-      <c r="ZX11" s="94" t="n"/>
-      <c r="ZY11" s="94" t="n"/>
-      <c r="ZZ11" s="94" t="n"/>
-      <c r="AAA11" s="94" t="n"/>
-      <c r="AAB11" s="95" t="n"/>
-      <c r="AAC11" s="95" t="n"/>
-      <c r="AAD11" s="95" t="n"/>
-      <c r="AAE11" s="95" t="n"/>
-      <c r="AAF11" s="95" t="n"/>
-      <c r="AAG11" s="95" t="n"/>
-      <c r="AAH11" s="95" t="n"/>
-      <c r="AAI11" s="95" t="n"/>
-      <c r="AAJ11" s="95" t="n"/>
-      <c r="AAK11" s="95" t="n"/>
-      <c r="AAL11" s="95" t="n"/>
-      <c r="AAM11" s="95" t="n"/>
-      <c r="AAN11" s="95" t="n"/>
-      <c r="AAO11" s="95" t="n"/>
-      <c r="AAP11" s="95" t="n"/>
-      <c r="AAQ11" s="95" t="n"/>
-      <c r="AAR11" s="95" t="n"/>
-      <c r="AAS11" s="95" t="n"/>
-      <c r="AAT11" s="95" t="n"/>
-      <c r="AAU11" s="95" t="n"/>
-      <c r="AAV11" s="95" t="n"/>
-      <c r="AAW11" s="95" t="n"/>
-      <c r="AAX11" s="95" t="n"/>
-      <c r="AAY11" s="95" t="n"/>
-      <c r="AAZ11" s="95" t="n"/>
-      <c r="ABA11" s="95" t="n"/>
-      <c r="ABB11" s="95" t="n"/>
-      <c r="ABC11" s="95" t="n"/>
-      <c r="ABD11" s="95" t="n"/>
-      <c r="ABE11" s="95" t="n"/>
-      <c r="ABF11" s="95" t="n"/>
-      <c r="ABG11" s="95" t="n"/>
-      <c r="ABH11" s="95" t="n"/>
-      <c r="ABI11" s="95" t="n"/>
-      <c r="ABJ11" s="95" t="n"/>
-      <c r="ABK11" s="95" t="n"/>
-      <c r="ABL11" s="95" t="n"/>
-      <c r="ABM11" s="95" t="n"/>
-      <c r="ABN11" s="95" t="n"/>
-      <c r="ABO11" s="95" t="n"/>
-      <c r="ABP11" s="95" t="n"/>
-      <c r="ABQ11" s="95" t="n"/>
-      <c r="ABR11" s="95" t="n"/>
-      <c r="ABS11" s="95" t="n"/>
-      <c r="ABT11" s="95" t="n"/>
-      <c r="ABU11" s="95" t="n"/>
-      <c r="ABV11" s="95" t="n"/>
-      <c r="ABW11" s="95" t="n"/>
-      <c r="ABX11" s="95" t="n"/>
-      <c r="ABY11" s="95" t="n"/>
-      <c r="ABZ11" s="95" t="n"/>
-      <c r="ACA11" s="95" t="n"/>
-      <c r="ACB11" s="95" t="n"/>
-      <c r="ACC11" s="95" t="n"/>
-      <c r="ACD11" s="95" t="n"/>
-      <c r="ACE11" s="95" t="n"/>
-      <c r="ACF11" s="95" t="n"/>
-      <c r="ACG11" s="95" t="n"/>
-      <c r="ACH11" s="95" t="n"/>
-      <c r="ACI11" s="95" t="n"/>
-      <c r="ACJ11" s="95" t="n"/>
-      <c r="ACK11" s="95" t="n"/>
-      <c r="ACL11" s="95" t="n"/>
-      <c r="ACM11" s="97" t="n"/>
-      <c r="ACN11" s="98" t="n"/>
-      <c r="ACO11" s="98" t="n"/>
-      <c r="ACP11" s="98" t="n"/>
-      <c r="ACQ11" s="98" t="n"/>
-      <c r="ACR11" s="99" t="n"/>
-      <c r="ACS11" s="97" t="n"/>
-      <c r="ACT11" s="98" t="n"/>
-      <c r="ACU11" s="98" t="n"/>
-      <c r="ACV11" s="98" t="n"/>
-      <c r="ACW11" s="98" t="n"/>
-      <c r="ACX11" s="99" t="n"/>
-      <c r="ACY11" s="96" t="n"/>
-      <c r="ACZ11" s="96" t="n"/>
-      <c r="ADA11" s="96" t="n"/>
-      <c r="ADB11" s="96" t="n"/>
+      <c r="XV11" s="109" t="n"/>
+      <c r="XW11" s="109" t="n"/>
+      <c r="XX11" s="109" t="n"/>
+      <c r="XY11" s="107" t="n"/>
+      <c r="XZ11" s="107" t="n"/>
+      <c r="YA11" s="107" t="n"/>
+      <c r="YB11" s="107" t="n"/>
+      <c r="YC11" s="107" t="n"/>
+      <c r="YD11" s="107" t="n"/>
+      <c r="YE11" s="107" t="n"/>
+      <c r="YF11" s="107" t="n"/>
+      <c r="YG11" s="107" t="n"/>
+      <c r="YH11" s="107" t="n"/>
+      <c r="YI11" s="107" t="n"/>
+      <c r="YJ11" s="107" t="n"/>
+      <c r="YK11" s="107" t="n"/>
+      <c r="YL11" s="107" t="n"/>
+      <c r="YM11" s="87" t="n"/>
+      <c r="YN11" s="87" t="n"/>
+      <c r="YO11" s="87" t="n"/>
+      <c r="YP11" s="87" t="n"/>
+      <c r="YQ11" s="87" t="n"/>
+      <c r="YR11" s="87" t="n"/>
+      <c r="YS11" s="87" t="n"/>
+      <c r="YT11" s="87" t="n"/>
+      <c r="YU11" s="87" t="n"/>
+      <c r="YV11" s="87" t="n"/>
+      <c r="YW11" s="87" t="n"/>
+      <c r="YX11" s="87" t="n"/>
+      <c r="YY11" s="87" t="n"/>
+      <c r="YZ11" s="87" t="n"/>
+      <c r="ZA11" s="87" t="n"/>
+      <c r="ZB11" s="87" t="n"/>
+      <c r="ZC11" s="87" t="n"/>
+      <c r="ZD11" s="87" t="n"/>
+      <c r="ZE11" s="87" t="n"/>
+      <c r="ZF11" s="87" t="n"/>
+      <c r="ZG11" s="87" t="n"/>
+      <c r="ZH11" s="88" t="n"/>
+      <c r="ZI11" s="88" t="n"/>
+      <c r="ZJ11" s="88" t="n"/>
+      <c r="ZK11" s="88" t="n"/>
+      <c r="ZL11" s="88" t="n"/>
+      <c r="ZM11" s="88" t="n"/>
+      <c r="ZN11" s="88" t="n"/>
+      <c r="ZO11" s="88" t="n"/>
+      <c r="ZP11" s="88" t="n"/>
+      <c r="ZQ11" s="88" t="n"/>
+      <c r="ZR11" s="88" t="n"/>
+      <c r="ZS11" s="88" t="n"/>
+      <c r="ZT11" s="88" t="n"/>
+      <c r="ZU11" s="88" t="n"/>
+      <c r="ZV11" s="88" t="n"/>
+      <c r="ZW11" s="88" t="n"/>
+      <c r="ZX11" s="88" t="n"/>
+      <c r="ZY11" s="88" t="n"/>
+      <c r="ZZ11" s="88" t="n"/>
+      <c r="AAA11" s="88" t="n"/>
+      <c r="AAB11" s="89" t="n"/>
+      <c r="AAC11" s="89" t="n"/>
+      <c r="AAD11" s="89" t="n"/>
+      <c r="AAE11" s="89" t="n"/>
+      <c r="AAF11" s="89" t="n"/>
+      <c r="AAG11" s="89" t="n"/>
+      <c r="AAH11" s="89" t="n"/>
+      <c r="AAI11" s="89" t="n"/>
+      <c r="AAJ11" s="89" t="n"/>
+      <c r="AAK11" s="89" t="n"/>
+      <c r="AAL11" s="89" t="n"/>
+      <c r="AAM11" s="89" t="n"/>
+      <c r="AAN11" s="89" t="n"/>
+      <c r="AAO11" s="89" t="n"/>
+      <c r="AAP11" s="89" t="n"/>
+      <c r="AAQ11" s="89" t="n"/>
+      <c r="AAR11" s="89" t="n"/>
+      <c r="AAS11" s="89" t="n"/>
+      <c r="AAT11" s="89" t="n"/>
+      <c r="AAU11" s="89" t="n"/>
+      <c r="AAV11" s="89" t="n"/>
+      <c r="AAW11" s="89" t="n"/>
+      <c r="AAX11" s="89" t="n"/>
+      <c r="AAY11" s="89" t="n"/>
+      <c r="AAZ11" s="89" t="n"/>
+      <c r="ABA11" s="89" t="n"/>
+      <c r="ABB11" s="89" t="n"/>
+      <c r="ABC11" s="89" t="n"/>
+      <c r="ABD11" s="89" t="n"/>
+      <c r="ABE11" s="89" t="n"/>
+      <c r="ABF11" s="89" t="n"/>
+      <c r="ABG11" s="89" t="n"/>
+      <c r="ABH11" s="89" t="n"/>
+      <c r="ABI11" s="89" t="n"/>
+      <c r="ABJ11" s="89" t="n"/>
+      <c r="ABK11" s="89" t="n"/>
+      <c r="ABL11" s="89" t="n"/>
+      <c r="ABM11" s="89" t="n"/>
+      <c r="ABN11" s="89" t="n"/>
+      <c r="ABO11" s="89" t="n"/>
+      <c r="ABP11" s="89" t="n"/>
+      <c r="ABQ11" s="89" t="n"/>
+      <c r="ABR11" s="89" t="n"/>
+      <c r="ABS11" s="89" t="n"/>
+      <c r="ABT11" s="89" t="n"/>
+      <c r="ABU11" s="89" t="n"/>
+      <c r="ABV11" s="89" t="n"/>
+      <c r="ABW11" s="89" t="n"/>
+      <c r="ABX11" s="89" t="n"/>
+      <c r="ABY11" s="89" t="n"/>
+      <c r="ABZ11" s="89" t="n"/>
+      <c r="ACA11" s="89" t="n"/>
+      <c r="ACB11" s="89" t="n"/>
+      <c r="ACC11" s="89" t="n"/>
+      <c r="ACD11" s="89" t="n"/>
+      <c r="ACE11" s="89" t="n"/>
+      <c r="ACF11" s="89" t="n"/>
+      <c r="ACG11" s="89" t="n"/>
+      <c r="ACH11" s="89" t="n"/>
+      <c r="ACI11" s="89" t="n"/>
+      <c r="ACJ11" s="89" t="n"/>
+      <c r="ACK11" s="89" t="n"/>
+      <c r="ACL11" s="89" t="n"/>
+      <c r="ACM11" s="91" t="n"/>
+      <c r="ACN11" s="92" t="n"/>
+      <c r="ACO11" s="92" t="n"/>
+      <c r="ACP11" s="92" t="n"/>
+      <c r="ACQ11" s="92" t="n"/>
+      <c r="ACR11" s="93" t="n"/>
+      <c r="ACS11" s="91" t="n"/>
+      <c r="ACT11" s="92" t="n"/>
+      <c r="ACU11" s="92" t="n"/>
+      <c r="ACV11" s="92" t="n"/>
+      <c r="ACW11" s="92" t="n"/>
+      <c r="ACX11" s="93" t="n"/>
+      <c r="ACY11" s="90" t="n"/>
+      <c r="ACZ11" s="90" t="n"/>
+      <c r="ADA11" s="90" t="n"/>
+      <c r="ADB11" s="90" t="n"/>
       <c r="ADC11" s="31" t="n"/>
       <c r="ADD11" s="31" t="n"/>
       <c r="ADE11" s="11" t="n"/>
@@ -55369,7 +55364,7 @@
       <c r="AJQ11" s="11" t="n"/>
       <c r="AJR11" s="11" t="n"/>
       <c r="AJS11" s="11" t="n"/>
-      <c r="AJT11" s="79" t="n"/>
+      <c r="AJT11" s="108" t="n"/>
       <c r="AJU11" s="11" t="n"/>
       <c r="AJV11" s="11" t="n"/>
       <c r="AJW11" s="11" t="n"/>
@@ -55385,74 +55380,74 @@
       <c r="AKG11" s="31" t="n"/>
       <c r="AKH11" s="31" t="n"/>
       <c r="AKI11" s="31" t="n"/>
-      <c r="AKJ11" s="100" t="n"/>
-      <c r="AKK11" s="105" t="n"/>
-      <c r="AKL11" s="106" t="n"/>
-      <c r="AKM11" s="106" t="n"/>
-      <c r="AKN11" s="106" t="n"/>
-      <c r="AKO11" s="107" t="n"/>
-      <c r="AKP11" s="101" t="n"/>
-      <c r="AKQ11" s="82" t="n"/>
-      <c r="AKR11" s="82" t="n"/>
-      <c r="AKS11" s="82" t="n"/>
-      <c r="AKT11" s="82" t="n"/>
-      <c r="AKU11" s="91" t="n"/>
-      <c r="AKV11" s="91" t="n"/>
-      <c r="AKW11" s="91" t="n"/>
-      <c r="AKX11" s="91" t="n"/>
-      <c r="AKY11" s="103" t="n"/>
-      <c r="AKZ11" s="104" t="n"/>
-      <c r="ALA11" s="104" t="n"/>
-      <c r="ALB11" s="104" t="n"/>
-      <c r="ALC11" s="104" t="n"/>
-      <c r="ALD11" s="104" t="n"/>
-      <c r="ALE11" s="104" t="n"/>
-      <c r="ALF11" s="102" t="n"/>
-      <c r="ALG11" s="102" t="n"/>
-      <c r="ALH11" s="104" t="n"/>
-      <c r="ALI11" s="102" t="n"/>
-      <c r="ALJ11" s="102" t="n"/>
-      <c r="ALK11" s="102" t="n"/>
-      <c r="ALL11" s="102" t="n"/>
-      <c r="ALM11" s="102" t="n"/>
-      <c r="ALN11" s="102" t="n"/>
-      <c r="ALO11" s="102" t="n"/>
-      <c r="ALP11" s="102" t="n"/>
-      <c r="ALQ11" s="102" t="n"/>
-      <c r="ALR11" s="102" t="n"/>
-      <c r="ALS11" s="102" t="n"/>
-      <c r="ALT11" s="102" t="n"/>
-      <c r="ALU11" s="102" t="n"/>
-      <c r="ALV11" s="102" t="n"/>
-      <c r="ALW11" s="102" t="n"/>
-      <c r="ALX11" s="102" t="n"/>
-      <c r="ALY11" s="102" t="n"/>
-      <c r="ALZ11" s="102" t="n"/>
-      <c r="AMA11" s="102" t="n"/>
-      <c r="AMB11" s="102" t="n"/>
-      <c r="AMC11" s="102" t="n"/>
-      <c r="AMD11" s="102" t="n"/>
-      <c r="AME11" s="102" t="n"/>
-      <c r="AMF11" s="102" t="n"/>
-      <c r="AMG11" s="102" t="n"/>
-      <c r="AMH11" s="102" t="n"/>
-      <c r="AMI11" s="102" t="n"/>
-      <c r="AMJ11" s="102" t="n"/>
-      <c r="AMK11" s="102" t="n"/>
-      <c r="AML11" s="102" t="n"/>
-      <c r="AMM11" s="102" t="n"/>
-      <c r="AMN11" s="102" t="n"/>
-      <c r="AMO11" s="102" t="n"/>
-      <c r="AMP11" s="102" t="n"/>
-      <c r="AMQ11" s="102" t="n"/>
-      <c r="AMR11" s="102" t="n"/>
-      <c r="AMS11" s="102" t="n"/>
-      <c r="AMT11" s="102" t="n"/>
-      <c r="AMU11" s="102" t="n"/>
-      <c r="AMV11" s="102" t="n"/>
-      <c r="AMW11" s="102" t="n"/>
-      <c r="AMX11" s="102" t="n"/>
-      <c r="AMY11" s="102" t="n"/>
+      <c r="AKJ11" s="94" t="n"/>
+      <c r="AKK11" s="99" t="n"/>
+      <c r="AKL11" s="100" t="n"/>
+      <c r="AKM11" s="100" t="n"/>
+      <c r="AKN11" s="100" t="n"/>
+      <c r="AKO11" s="101" t="n"/>
+      <c r="AKP11" s="95" t="n"/>
+      <c r="AKQ11" s="109" t="n"/>
+      <c r="AKR11" s="109" t="n"/>
+      <c r="AKS11" s="109" t="n"/>
+      <c r="AKT11" s="109" t="n"/>
+      <c r="AKU11" s="85" t="n"/>
+      <c r="AKV11" s="85" t="n"/>
+      <c r="AKW11" s="85" t="n"/>
+      <c r="AKX11" s="85" t="n"/>
+      <c r="AKY11" s="97" t="n"/>
+      <c r="AKZ11" s="98" t="n"/>
+      <c r="ALA11" s="98" t="n"/>
+      <c r="ALB11" s="98" t="n"/>
+      <c r="ALC11" s="98" t="n"/>
+      <c r="ALD11" s="98" t="n"/>
+      <c r="ALE11" s="98" t="n"/>
+      <c r="ALF11" s="96" t="n"/>
+      <c r="ALG11" s="96" t="n"/>
+      <c r="ALH11" s="98" t="n"/>
+      <c r="ALI11" s="96" t="n"/>
+      <c r="ALJ11" s="96" t="n"/>
+      <c r="ALK11" s="96" t="n"/>
+      <c r="ALL11" s="96" t="n"/>
+      <c r="ALM11" s="96" t="n"/>
+      <c r="ALN11" s="96" t="n"/>
+      <c r="ALO11" s="96" t="n"/>
+      <c r="ALP11" s="96" t="n"/>
+      <c r="ALQ11" s="96" t="n"/>
+      <c r="ALR11" s="96" t="n"/>
+      <c r="ALS11" s="96" t="n"/>
+      <c r="ALT11" s="96" t="n"/>
+      <c r="ALU11" s="96" t="n"/>
+      <c r="ALV11" s="96" t="n"/>
+      <c r="ALW11" s="96" t="n"/>
+      <c r="ALX11" s="96" t="n"/>
+      <c r="ALY11" s="96" t="n"/>
+      <c r="ALZ11" s="96" t="n"/>
+      <c r="AMA11" s="96" t="n"/>
+      <c r="AMB11" s="96" t="n"/>
+      <c r="AMC11" s="96" t="n"/>
+      <c r="AMD11" s="96" t="n"/>
+      <c r="AME11" s="96" t="n"/>
+      <c r="AMF11" s="96" t="n"/>
+      <c r="AMG11" s="96" t="n"/>
+      <c r="AMH11" s="96" t="n"/>
+      <c r="AMI11" s="96" t="n"/>
+      <c r="AMJ11" s="96" t="n"/>
+      <c r="AMK11" s="96" t="n"/>
+      <c r="AML11" s="96" t="n"/>
+      <c r="AMM11" s="96" t="n"/>
+      <c r="AMN11" s="96" t="n"/>
+      <c r="AMO11" s="96" t="n"/>
+      <c r="AMP11" s="96" t="n"/>
+      <c r="AMQ11" s="96" t="n"/>
+      <c r="AMR11" s="96" t="n"/>
+      <c r="AMS11" s="96" t="n"/>
+      <c r="AMT11" s="96" t="n"/>
+      <c r="AMU11" s="96" t="n"/>
+      <c r="AMV11" s="96" t="n"/>
+      <c r="AMW11" s="96" t="n"/>
+      <c r="AMX11" s="96" t="n"/>
+      <c r="AMY11" s="96" t="n"/>
       <c r="AON11" s="20" t="inlineStr">
         <is>
           <t>Induction</t>
@@ -55611,7 +55606,7 @@
           <t>On</t>
         </is>
       </c>
-      <c r="APT11" s="108" t="inlineStr">
+      <c r="APT11" s="102" t="inlineStr">
         <is>
           <t>WOH Training</t>
         </is>
@@ -56025,16 +56020,18 @@
     <row r="12" ht="15.6" customHeight="1">
       <c r="A12" s="77" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>Site Manager</t>
         </is>
       </c>
       <c r="B12" s="78" t="inlineStr">
         <is>
-          <t>Aldair Hernandez</t>
-        </is>
-      </c>
-      <c r="C12" s="74" t="n">
-        <v>123456789</v>
+          <t>Miguel Venegas</t>
+        </is>
+      </c>
+      <c r="C12" s="74" t="inlineStr">
+        <is>
+          <t>TP0352</t>
+        </is>
       </c>
       <c r="ARB12" s="84" t="inlineStr">
         <is>
@@ -56107,6 +56104,46 @@
         </is>
       </c>
       <c r="ARP12" s="84" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARZ12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASA12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASB12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASC12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASD12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASE12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASF12" s="103" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASG12" s="103" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
@@ -56115,134 +56152,42 @@
     <row r="13" ht="15.6" customHeight="1">
       <c r="A13" s="77" t="inlineStr">
         <is>
-          <t>Site Manager</t>
+          <t>Data Analyst</t>
         </is>
       </c>
       <c r="B13" s="78" t="inlineStr">
         <is>
-          <t>Miguel Venegas</t>
+          <t>Jose Gomez</t>
         </is>
       </c>
       <c r="C13" s="74" t="inlineStr">
         <is>
-          <t>TP0352</t>
-        </is>
-      </c>
-      <c r="ARB13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARC13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARD13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARE13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARF13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARG13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARH13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARI13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARJ13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARK13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARL13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARM13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARN13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARO13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARP13" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARZ13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASA13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASB13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASC13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASD13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASE13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASF13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASG13" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>TP0039</t>
+        </is>
+      </c>
+      <c r="ARB13" s="84" t="n"/>
+      <c r="ARC13" s="84" t="n"/>
+      <c r="ARD13" s="84" t="n"/>
+      <c r="ARE13" s="84" t="n"/>
+      <c r="ARF13" s="84" t="n"/>
+      <c r="ARG13" s="84" t="n"/>
+      <c r="ARH13" s="84" t="n"/>
+      <c r="ARI13" s="84" t="n"/>
+      <c r="ARJ13" s="84" t="n"/>
+      <c r="ARK13" s="84" t="n"/>
+      <c r="ARL13" s="84" t="n"/>
+      <c r="ARM13" s="84" t="n"/>
+      <c r="ARN13" s="84" t="n"/>
+      <c r="ARO13" s="84" t="n"/>
+      <c r="ARP13" s="84" t="n"/>
+      <c r="ARZ13" s="103" t="n"/>
+      <c r="ASA13" s="103" t="n"/>
+      <c r="ASB13" s="103" t="n"/>
+      <c r="ASC13" s="103" t="n"/>
+      <c r="ASD13" s="103" t="n"/>
+      <c r="ASE13" s="103" t="n"/>
+      <c r="ASF13" s="103" t="n"/>
+      <c r="ASG13" s="103" t="n"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -56252,7 +56197,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Elver Gonzales</t>
+          <t xml:space="preserve">Vincent Rolong </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -56260,171 +56205,74 @@
           <t>12345678</t>
         </is>
       </c>
-      <c r="ARE14" s="111" t="inlineStr">
+      <c r="ARG14" s="110" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARF14" s="111" t="inlineStr">
+      <c r="ARH14" s="110" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARG14" s="111" t="inlineStr">
+      <c r="ARI14" s="110" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARH14" s="111" t="inlineStr">
+      <c r="ARJ14" s="110" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARI14" s="111" t="inlineStr">
+      <c r="ARK14" s="110" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARJ14" s="111" t="inlineStr">
+      <c r="ARL14" s="110" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARK14" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARL14" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARM14" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
       <c r="ARN14" s="111" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>ON NS</t>
         </is>
       </c>
       <c r="ARO14" s="111" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>ON NS</t>
         </is>
       </c>
       <c r="ARP14" s="111" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>ON NS</t>
         </is>
       </c>
       <c r="ARQ14" s="111" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>ON NS</t>
         </is>
       </c>
       <c r="ARR14" s="111" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>ON NS</t>
         </is>
       </c>
       <c r="ARS14" s="111" t="inlineStr">
         <is>
-          <t>ON</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Data Analyst</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Roberto Angulo</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>98787654321</t>
-        </is>
-      </c>
-      <c r="ARE15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARF15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARG15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARH15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARI15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARJ15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARK15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARL15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARM15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARN15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARO15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARP15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARQ15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARR15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARS15" s="111" t="inlineStr">
-        <is>
-          <t>ON</t>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ART14" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARU14" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se realiza correccion del problema de UI/UX donde se salian la ultima fila no se apreciaba
</commit_message>
<xml_diff>
--- a/PlanStaff.xlsx
+++ b/PlanStaff.xlsx
@@ -73,7 +73,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="45">
     <fill>
       <patternFill/>
     </fill>
@@ -304,12 +304,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -330,12 +324,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor rgb="FFA8D08D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -464,7 +452,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -700,29 +688,16 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="46" fontId="5" fillId="39" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="46" fontId="5" fillId="40" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="41" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="42" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -749,13 +724,13 @@
     <xf numFmtId="46" fontId="5" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="40" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="46" fontId="5" fillId="39" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="40" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="46" fontId="5" fillId="39" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="40" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="46" fontId="5" fillId="39" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="46" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -767,10 +742,21 @@
     <xf numFmtId="46" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="43" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="46" fontId="5" fillId="42" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -785,8 +771,8 @@
     <xf numFmtId="46" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1267,14 +1253,14 @@
   </sheetPr>
   <dimension ref="A1:AWU14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="16" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="29.77734375" bestFit="1" customWidth="1" style="83" min="2" max="2"/>
+    <col width="29.77734375" bestFit="1" customWidth="1" style="79" min="2" max="2"/>
     <col width="16.21875" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -19217,7 +19203,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="OP4" s="108" t="inlineStr">
+      <c r="OP4" s="106" t="inlineStr">
         <is>
           <t>On call NS</t>
         </is>
@@ -19597,7 +19583,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="RN4" s="108" t="inlineStr">
+      <c r="RN4" s="106" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
@@ -20462,7 +20448,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="YE4" s="108" t="n"/>
+      <c r="YE4" s="106" t="n"/>
       <c r="YF4" s="10" t="inlineStr">
         <is>
           <t>On</t>
@@ -20563,7 +20549,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="YZ4" s="108" t="inlineStr">
+      <c r="YZ4" s="106" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
@@ -21088,7 +21074,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ADA4" s="108" t="inlineStr">
+      <c r="ADA4" s="106" t="inlineStr">
         <is>
           <t>Transition</t>
         </is>
@@ -21508,7 +21494,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AGG4" s="108" t="inlineStr">
+      <c r="AGG4" s="106" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
@@ -21588,7 +21574,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AGW4" s="108" t="inlineStr">
+      <c r="AGW4" s="106" t="inlineStr">
         <is>
           <t>change</t>
         </is>
@@ -22068,7 +22054,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AKO4" s="109" t="inlineStr">
+      <c r="AKO4" s="107" t="inlineStr">
         <is>
           <t>On call NS</t>
         </is>
@@ -26316,7 +26302,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="XJ5" s="108" t="n"/>
+      <c r="XJ5" s="106" t="n"/>
       <c r="XK5" s="10" t="inlineStr">
         <is>
           <t>Night</t>
@@ -26942,7 +26928,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ACF5" s="107" t="n"/>
+      <c r="ACF5" s="105" t="n"/>
       <c r="ACG5" s="10" t="inlineStr">
         <is>
           <t>On</t>
@@ -28093,7 +28079,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="ALC5" s="109" t="inlineStr">
+      <c r="ALC5" s="107" t="inlineStr">
         <is>
           <t>On call NS</t>
         </is>
@@ -35719,7 +35705,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="FZ7" s="109" t="n"/>
+      <c r="FZ7" s="107" t="n"/>
       <c r="GA7" s="10" t="inlineStr">
         <is>
           <t>Day</t>
@@ -37704,15 +37690,15 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="XG7" s="108" t="inlineStr">
+      <c r="XG7" s="106" t="inlineStr">
         <is>
           <t>BAITALI FUEL TRUCK</t>
         </is>
       </c>
-      <c r="XH7" s="105" t="n"/>
-      <c r="XI7" s="105" t="n"/>
-      <c r="XJ7" s="105" t="n"/>
-      <c r="XK7" s="106" t="n"/>
+      <c r="XH7" s="103" t="n"/>
+      <c r="XI7" s="103" t="n"/>
+      <c r="XJ7" s="103" t="n"/>
+      <c r="XK7" s="104" t="n"/>
       <c r="XL7" s="11" t="inlineStr">
         <is>
           <t>Off</t>
@@ -37723,15 +37709,15 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="XN7" s="109" t="inlineStr">
+      <c r="XN7" s="107" t="inlineStr">
         <is>
           <t>BAITALI FUEL TRUCK and Waiting docs for HR induction</t>
         </is>
       </c>
-      <c r="XO7" s="105" t="n"/>
-      <c r="XP7" s="105" t="n"/>
-      <c r="XQ7" s="105" t="n"/>
-      <c r="XR7" s="106" t="n"/>
+      <c r="XO7" s="103" t="n"/>
+      <c r="XP7" s="103" t="n"/>
+      <c r="XQ7" s="103" t="n"/>
+      <c r="XR7" s="104" t="n"/>
       <c r="XS7" s="11" t="inlineStr">
         <is>
           <t>Off</t>
@@ -37742,71 +37728,71 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="XU7" s="107" t="inlineStr">
+      <c r="XU7" s="105" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="XV7" s="105" t="n"/>
-      <c r="XW7" s="105" t="n"/>
-      <c r="XX7" s="105" t="n"/>
-      <c r="XY7" s="106" t="n"/>
-      <c r="XZ7" s="107" t="inlineStr">
+      <c r="XV7" s="103" t="n"/>
+      <c r="XW7" s="103" t="n"/>
+      <c r="XX7" s="103" t="n"/>
+      <c r="XY7" s="104" t="n"/>
+      <c r="XZ7" s="105" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YA7" s="105" t="n"/>
-      <c r="YB7" s="105" t="n"/>
-      <c r="YC7" s="105" t="n"/>
-      <c r="YD7" s="106" t="n"/>
-      <c r="YE7" s="107" t="inlineStr">
+      <c r="YA7" s="103" t="n"/>
+      <c r="YB7" s="103" t="n"/>
+      <c r="YC7" s="103" t="n"/>
+      <c r="YD7" s="104" t="n"/>
+      <c r="YE7" s="105" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YF7" s="105" t="n"/>
-      <c r="YG7" s="105" t="n"/>
-      <c r="YH7" s="105" t="n"/>
-      <c r="YI7" s="106" t="n"/>
-      <c r="YJ7" s="107" t="inlineStr">
+      <c r="YF7" s="103" t="n"/>
+      <c r="YG7" s="103" t="n"/>
+      <c r="YH7" s="103" t="n"/>
+      <c r="YI7" s="104" t="n"/>
+      <c r="YJ7" s="105" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YK7" s="105" t="n"/>
-      <c r="YL7" s="105" t="n"/>
-      <c r="YM7" s="105" t="n"/>
-      <c r="YN7" s="106" t="n"/>
-      <c r="YO7" s="104" t="inlineStr">
+      <c r="YK7" s="103" t="n"/>
+      <c r="YL7" s="103" t="n"/>
+      <c r="YM7" s="103" t="n"/>
+      <c r="YN7" s="104" t="n"/>
+      <c r="YO7" s="102" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YP7" s="105" t="n"/>
-      <c r="YQ7" s="105" t="n"/>
-      <c r="YR7" s="105" t="n"/>
-      <c r="YS7" s="106" t="n"/>
-      <c r="YT7" s="104" t="inlineStr">
+      <c r="YP7" s="103" t="n"/>
+      <c r="YQ7" s="103" t="n"/>
+      <c r="YR7" s="103" t="n"/>
+      <c r="YS7" s="104" t="n"/>
+      <c r="YT7" s="102" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YU7" s="105" t="n"/>
-      <c r="YV7" s="105" t="n"/>
-      <c r="YW7" s="105" t="n"/>
-      <c r="YX7" s="106" t="n"/>
-      <c r="YY7" s="104" t="inlineStr">
+      <c r="YU7" s="103" t="n"/>
+      <c r="YV7" s="103" t="n"/>
+      <c r="YW7" s="103" t="n"/>
+      <c r="YX7" s="104" t="n"/>
+      <c r="YY7" s="102" t="inlineStr">
         <is>
           <t>Supporting Parbo Projects</t>
         </is>
       </c>
-      <c r="YZ7" s="105" t="n"/>
-      <c r="ZA7" s="105" t="n"/>
-      <c r="ZB7" s="105" t="n"/>
-      <c r="ZC7" s="105" t="n"/>
-      <c r="ZD7" s="106" t="n"/>
-      <c r="ZE7" s="104" t="inlineStr">
+      <c r="YZ7" s="103" t="n"/>
+      <c r="ZA7" s="103" t="n"/>
+      <c r="ZB7" s="103" t="n"/>
+      <c r="ZC7" s="103" t="n"/>
+      <c r="ZD7" s="104" t="n"/>
+      <c r="ZE7" s="102" t="inlineStr">
         <is>
           <t>RGM HR</t>
         </is>
@@ -38246,7 +38232,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ACO7" s="108" t="n"/>
+      <c r="ACO7" s="106" t="n"/>
       <c r="ACP7" s="10" t="inlineStr">
         <is>
           <t>On</t>
@@ -43000,7 +42986,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="TH8" s="108" t="n"/>
+      <c r="TH8" s="106" t="n"/>
       <c r="TI8" s="10" t="inlineStr">
         <is>
           <t>Day</t>
@@ -48548,7 +48534,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="QC9" s="108" t="n"/>
+      <c r="QC9" s="106" t="n"/>
       <c r="QD9" s="10" t="inlineStr">
         <is>
           <t>Day</t>
@@ -50329,7 +50315,7 @@
           <t>night</t>
         </is>
       </c>
-      <c r="ADV9" s="108" t="inlineStr">
+      <c r="ADV9" s="106" t="inlineStr">
         <is>
           <t>Transitio</t>
         </is>
@@ -51139,7 +51125,7 @@
           <t>FA night</t>
         </is>
       </c>
-      <c r="AKB9" s="108" t="inlineStr">
+      <c r="AKB9" s="106" t="inlineStr">
         <is>
           <t>On call</t>
         </is>
@@ -52252,13 +52238,13 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="ASX9" s="108" t="n"/>
-      <c r="ASY9" s="108" t="n"/>
-      <c r="ASZ9" s="108" t="n"/>
-      <c r="ATA9" s="108" t="n"/>
-      <c r="ATB9" s="108" t="n"/>
-      <c r="ATC9" s="108" t="n"/>
-      <c r="ATD9" s="108" t="n"/>
+      <c r="ASX9" s="106" t="n"/>
+      <c r="ASY9" s="106" t="n"/>
+      <c r="ASZ9" s="106" t="n"/>
+      <c r="ATA9" s="106" t="n"/>
+      <c r="ATB9" s="106" t="n"/>
+      <c r="ATC9" s="106" t="n"/>
+      <c r="ATD9" s="106" t="n"/>
     </row>
     <row r="10" ht="30" customFormat="1" customHeight="1" s="8">
       <c r="A10" s="77" t="inlineStr">
@@ -53040,7 +53026,7 @@
       <c r="ACK10" s="29" t="n"/>
       <c r="ACL10" s="29" t="n"/>
       <c r="ACM10" s="31" t="n"/>
-      <c r="ACN10" s="109" t="n"/>
+      <c r="ACN10" s="107" t="n"/>
       <c r="ACO10" s="31" t="n"/>
       <c r="ACP10" s="31" t="n"/>
       <c r="ACQ10" s="31" t="n"/>
@@ -53163,15 +53149,15 @@
       <c r="AHD10" s="45" t="n"/>
       <c r="AHE10" s="45" t="n"/>
       <c r="AHF10" s="45" t="n"/>
-      <c r="AHG10" s="109" t="n"/>
-      <c r="AHH10" s="109" t="n"/>
-      <c r="AHI10" s="109" t="n"/>
-      <c r="AHJ10" s="109" t="n"/>
-      <c r="AHK10" s="109" t="n"/>
-      <c r="AHL10" s="109" t="n"/>
-      <c r="AHM10" s="109" t="n"/>
-      <c r="AHN10" s="109" t="n"/>
-      <c r="AHO10" s="109" t="n"/>
+      <c r="AHG10" s="107" t="n"/>
+      <c r="AHH10" s="107" t="n"/>
+      <c r="AHI10" s="107" t="n"/>
+      <c r="AHJ10" s="107" t="n"/>
+      <c r="AHK10" s="107" t="n"/>
+      <c r="AHL10" s="107" t="n"/>
+      <c r="AHM10" s="107" t="n"/>
+      <c r="AHN10" s="107" t="n"/>
+      <c r="AHO10" s="107" t="n"/>
       <c r="AHP10" s="42" t="n"/>
       <c r="AHQ10" s="42" t="n"/>
       <c r="AHR10" s="42" t="n"/>
@@ -53225,27 +53211,27 @@
       <c r="AJN10" s="42" t="n"/>
       <c r="AJO10" s="42" t="n"/>
       <c r="AJP10" s="42" t="n"/>
-      <c r="AJQ10" s="108" t="inlineStr">
+      <c r="AJQ10" s="106" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJR10" s="108" t="inlineStr">
+      <c r="AJR10" s="106" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJS10" s="108" t="inlineStr">
+      <c r="AJS10" s="106" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJT10" s="108" t="inlineStr">
+      <c r="AJT10" s="106" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
       </c>
-      <c r="AJU10" s="108" t="inlineStr">
+      <c r="AJU10" s="106" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
@@ -53260,7 +53246,7 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="AJX10" s="108" t="inlineStr">
+      <c r="AJX10" s="106" t="inlineStr">
         <is>
           <t>Fusecon</t>
         </is>
@@ -54951,83 +54937,83 @@
       <c r="TT11" s="42" t="n"/>
       <c r="TU11" s="42" t="n"/>
       <c r="TV11" s="42" t="n"/>
-      <c r="TW11" s="109" t="n"/>
-      <c r="TX11" s="109" t="n"/>
+      <c r="TW11" s="107" t="n"/>
+      <c r="TX11" s="107" t="n"/>
       <c r="TY11" s="11" t="n"/>
       <c r="TZ11" s="11" t="n"/>
-      <c r="UA11" s="109" t="n"/>
-      <c r="UB11" s="109" t="n"/>
-      <c r="UC11" s="109" t="n"/>
-      <c r="UD11" s="109" t="n"/>
-      <c r="UE11" s="109" t="n"/>
-      <c r="UF11" s="109" t="n"/>
-      <c r="UG11" s="109" t="n"/>
-      <c r="UH11" s="109" t="n"/>
-      <c r="UI11" s="109" t="n"/>
-      <c r="UJ11" s="109" t="n"/>
+      <c r="UA11" s="107" t="n"/>
+      <c r="UB11" s="107" t="n"/>
+      <c r="UC11" s="107" t="n"/>
+      <c r="UD11" s="107" t="n"/>
+      <c r="UE11" s="107" t="n"/>
+      <c r="UF11" s="107" t="n"/>
+      <c r="UG11" s="107" t="n"/>
+      <c r="UH11" s="107" t="n"/>
+      <c r="UI11" s="107" t="n"/>
+      <c r="UJ11" s="107" t="n"/>
       <c r="UK11" s="31" t="n"/>
       <c r="UL11" s="31" t="n"/>
       <c r="UM11" s="31" t="n"/>
       <c r="UN11" s="31" t="n"/>
-      <c r="UO11" s="86" t="n"/>
-      <c r="UP11" s="86" t="n"/>
-      <c r="UQ11" s="86" t="n"/>
-      <c r="UR11" s="86" t="n"/>
-      <c r="US11" s="86" t="n"/>
-      <c r="UT11" s="86" t="n"/>
-      <c r="UU11" s="86" t="n"/>
-      <c r="UV11" s="86" t="n"/>
-      <c r="UW11" s="86" t="n"/>
-      <c r="UX11" s="86" t="n"/>
-      <c r="UY11" s="86" t="n"/>
-      <c r="UZ11" s="86" t="n"/>
-      <c r="VA11" s="86" t="n"/>
-      <c r="VB11" s="86" t="n"/>
-      <c r="VC11" s="86" t="n"/>
-      <c r="VD11" s="86" t="n"/>
-      <c r="VE11" s="86" t="n"/>
-      <c r="VF11" s="86" t="n"/>
-      <c r="VG11" s="86" t="n"/>
-      <c r="VH11" s="86" t="n"/>
-      <c r="VI11" s="86" t="n"/>
-      <c r="VJ11" s="86" t="n"/>
-      <c r="VK11" s="86" t="n"/>
-      <c r="VL11" s="86" t="n"/>
-      <c r="VM11" s="86" t="n"/>
-      <c r="VN11" s="86" t="n"/>
-      <c r="VO11" s="86" t="n"/>
-      <c r="VP11" s="86" t="n"/>
-      <c r="VQ11" s="86" t="n"/>
-      <c r="VR11" s="86" t="n"/>
-      <c r="VS11" s="86" t="n"/>
-      <c r="VT11" s="86" t="n"/>
-      <c r="VU11" s="86" t="n"/>
-      <c r="VV11" s="86" t="n"/>
-      <c r="VW11" s="86" t="n"/>
-      <c r="VX11" s="86" t="n"/>
-      <c r="VY11" s="86" t="n"/>
-      <c r="VZ11" s="86" t="n"/>
-      <c r="WA11" s="86" t="n"/>
-      <c r="WB11" s="86" t="n"/>
-      <c r="WC11" s="86" t="n"/>
-      <c r="WD11" s="86" t="n"/>
-      <c r="WE11" s="86" t="n"/>
-      <c r="WF11" s="86" t="n"/>
-      <c r="WG11" s="86" t="n"/>
-      <c r="WH11" s="86" t="n"/>
-      <c r="WI11" s="86" t="n"/>
-      <c r="WJ11" s="86" t="n"/>
-      <c r="WK11" s="86" t="n"/>
-      <c r="WL11" s="86" t="n"/>
-      <c r="WM11" s="86" t="n"/>
-      <c r="WN11" s="86" t="n"/>
-      <c r="WO11" s="86" t="n"/>
-      <c r="WP11" s="86" t="n"/>
-      <c r="WQ11" s="86" t="n"/>
-      <c r="WR11" s="86" t="n"/>
-      <c r="WS11" s="86" t="n"/>
-      <c r="WT11" s="86" t="n"/>
-      <c r="WU11" s="86" t="n"/>
+      <c r="UO11" s="81" t="n"/>
+      <c r="UP11" s="81" t="n"/>
+      <c r="UQ11" s="81" t="n"/>
+      <c r="UR11" s="81" t="n"/>
+      <c r="US11" s="81" t="n"/>
+      <c r="UT11" s="81" t="n"/>
+      <c r="UU11" s="81" t="n"/>
+      <c r="UV11" s="81" t="n"/>
+      <c r="UW11" s="81" t="n"/>
+      <c r="UX11" s="81" t="n"/>
+      <c r="UY11" s="81" t="n"/>
+      <c r="UZ11" s="81" t="n"/>
+      <c r="VA11" s="81" t="n"/>
+      <c r="VB11" s="81" t="n"/>
+      <c r="VC11" s="81" t="n"/>
+      <c r="VD11" s="81" t="n"/>
+      <c r="VE11" s="81" t="n"/>
+      <c r="VF11" s="81" t="n"/>
+      <c r="VG11" s="81" t="n"/>
+      <c r="VH11" s="81" t="n"/>
+      <c r="VI11" s="81" t="n"/>
+      <c r="VJ11" s="81" t="n"/>
+      <c r="VK11" s="81" t="n"/>
+      <c r="VL11" s="81" t="n"/>
+      <c r="VM11" s="81" t="n"/>
+      <c r="VN11" s="81" t="n"/>
+      <c r="VO11" s="81" t="n"/>
+      <c r="VP11" s="81" t="n"/>
+      <c r="VQ11" s="81" t="n"/>
+      <c r="VR11" s="81" t="n"/>
+      <c r="VS11" s="81" t="n"/>
+      <c r="VT11" s="81" t="n"/>
+      <c r="VU11" s="81" t="n"/>
+      <c r="VV11" s="81" t="n"/>
+      <c r="VW11" s="81" t="n"/>
+      <c r="VX11" s="81" t="n"/>
+      <c r="VY11" s="81" t="n"/>
+      <c r="VZ11" s="81" t="n"/>
+      <c r="WA11" s="81" t="n"/>
+      <c r="WB11" s="81" t="n"/>
+      <c r="WC11" s="81" t="n"/>
+      <c r="WD11" s="81" t="n"/>
+      <c r="WE11" s="81" t="n"/>
+      <c r="WF11" s="81" t="n"/>
+      <c r="WG11" s="81" t="n"/>
+      <c r="WH11" s="81" t="n"/>
+      <c r="WI11" s="81" t="n"/>
+      <c r="WJ11" s="81" t="n"/>
+      <c r="WK11" s="81" t="n"/>
+      <c r="WL11" s="81" t="n"/>
+      <c r="WM11" s="81" t="n"/>
+      <c r="WN11" s="81" t="n"/>
+      <c r="WO11" s="81" t="n"/>
+      <c r="WP11" s="81" t="n"/>
+      <c r="WQ11" s="81" t="n"/>
+      <c r="WR11" s="81" t="n"/>
+      <c r="WS11" s="81" t="n"/>
+      <c r="WT11" s="81" t="n"/>
+      <c r="WU11" s="81" t="n"/>
       <c r="WV11" s="42" t="n"/>
       <c r="WW11" s="42" t="n"/>
       <c r="WX11" s="42" t="n"/>
@@ -55054,143 +55040,143 @@
       <c r="XS11" s="42" t="n"/>
       <c r="XT11" s="42" t="n"/>
       <c r="XU11" s="42" t="n"/>
-      <c r="XV11" s="109" t="n"/>
-      <c r="XW11" s="109" t="n"/>
-      <c r="XX11" s="109" t="n"/>
-      <c r="XY11" s="107" t="n"/>
-      <c r="XZ11" s="107" t="n"/>
-      <c r="YA11" s="107" t="n"/>
-      <c r="YB11" s="107" t="n"/>
-      <c r="YC11" s="107" t="n"/>
-      <c r="YD11" s="107" t="n"/>
-      <c r="YE11" s="107" t="n"/>
-      <c r="YF11" s="107" t="n"/>
-      <c r="YG11" s="107" t="n"/>
-      <c r="YH11" s="107" t="n"/>
-      <c r="YI11" s="107" t="n"/>
-      <c r="YJ11" s="107" t="n"/>
-      <c r="YK11" s="107" t="n"/>
-      <c r="YL11" s="107" t="n"/>
-      <c r="YM11" s="87" t="n"/>
-      <c r="YN11" s="87" t="n"/>
-      <c r="YO11" s="87" t="n"/>
-      <c r="YP11" s="87" t="n"/>
-      <c r="YQ11" s="87" t="n"/>
-      <c r="YR11" s="87" t="n"/>
-      <c r="YS11" s="87" t="n"/>
-      <c r="YT11" s="87" t="n"/>
-      <c r="YU11" s="87" t="n"/>
-      <c r="YV11" s="87" t="n"/>
-      <c r="YW11" s="87" t="n"/>
-      <c r="YX11" s="87" t="n"/>
-      <c r="YY11" s="87" t="n"/>
-      <c r="YZ11" s="87" t="n"/>
-      <c r="ZA11" s="87" t="n"/>
-      <c r="ZB11" s="87" t="n"/>
-      <c r="ZC11" s="87" t="n"/>
-      <c r="ZD11" s="87" t="n"/>
-      <c r="ZE11" s="87" t="n"/>
-      <c r="ZF11" s="87" t="n"/>
-      <c r="ZG11" s="87" t="n"/>
-      <c r="ZH11" s="88" t="n"/>
-      <c r="ZI11" s="88" t="n"/>
-      <c r="ZJ11" s="88" t="n"/>
-      <c r="ZK11" s="88" t="n"/>
-      <c r="ZL11" s="88" t="n"/>
-      <c r="ZM11" s="88" t="n"/>
-      <c r="ZN11" s="88" t="n"/>
-      <c r="ZO11" s="88" t="n"/>
-      <c r="ZP11" s="88" t="n"/>
-      <c r="ZQ11" s="88" t="n"/>
-      <c r="ZR11" s="88" t="n"/>
-      <c r="ZS11" s="88" t="n"/>
-      <c r="ZT11" s="88" t="n"/>
-      <c r="ZU11" s="88" t="n"/>
-      <c r="ZV11" s="88" t="n"/>
-      <c r="ZW11" s="88" t="n"/>
-      <c r="ZX11" s="88" t="n"/>
-      <c r="ZY11" s="88" t="n"/>
-      <c r="ZZ11" s="88" t="n"/>
-      <c r="AAA11" s="88" t="n"/>
-      <c r="AAB11" s="89" t="n"/>
-      <c r="AAC11" s="89" t="n"/>
-      <c r="AAD11" s="89" t="n"/>
-      <c r="AAE11" s="89" t="n"/>
-      <c r="AAF11" s="89" t="n"/>
-      <c r="AAG11" s="89" t="n"/>
-      <c r="AAH11" s="89" t="n"/>
-      <c r="AAI11" s="89" t="n"/>
-      <c r="AAJ11" s="89" t="n"/>
-      <c r="AAK11" s="89" t="n"/>
-      <c r="AAL11" s="89" t="n"/>
-      <c r="AAM11" s="89" t="n"/>
-      <c r="AAN11" s="89" t="n"/>
-      <c r="AAO11" s="89" t="n"/>
-      <c r="AAP11" s="89" t="n"/>
-      <c r="AAQ11" s="89" t="n"/>
-      <c r="AAR11" s="89" t="n"/>
-      <c r="AAS11" s="89" t="n"/>
-      <c r="AAT11" s="89" t="n"/>
-      <c r="AAU11" s="89" t="n"/>
-      <c r="AAV11" s="89" t="n"/>
-      <c r="AAW11" s="89" t="n"/>
-      <c r="AAX11" s="89" t="n"/>
-      <c r="AAY11" s="89" t="n"/>
-      <c r="AAZ11" s="89" t="n"/>
-      <c r="ABA11" s="89" t="n"/>
-      <c r="ABB11" s="89" t="n"/>
-      <c r="ABC11" s="89" t="n"/>
-      <c r="ABD11" s="89" t="n"/>
-      <c r="ABE11" s="89" t="n"/>
-      <c r="ABF11" s="89" t="n"/>
-      <c r="ABG11" s="89" t="n"/>
-      <c r="ABH11" s="89" t="n"/>
-      <c r="ABI11" s="89" t="n"/>
-      <c r="ABJ11" s="89" t="n"/>
-      <c r="ABK11" s="89" t="n"/>
-      <c r="ABL11" s="89" t="n"/>
-      <c r="ABM11" s="89" t="n"/>
-      <c r="ABN11" s="89" t="n"/>
-      <c r="ABO11" s="89" t="n"/>
-      <c r="ABP11" s="89" t="n"/>
-      <c r="ABQ11" s="89" t="n"/>
-      <c r="ABR11" s="89" t="n"/>
-      <c r="ABS11" s="89" t="n"/>
-      <c r="ABT11" s="89" t="n"/>
-      <c r="ABU11" s="89" t="n"/>
-      <c r="ABV11" s="89" t="n"/>
-      <c r="ABW11" s="89" t="n"/>
-      <c r="ABX11" s="89" t="n"/>
-      <c r="ABY11" s="89" t="n"/>
-      <c r="ABZ11" s="89" t="n"/>
-      <c r="ACA11" s="89" t="n"/>
-      <c r="ACB11" s="89" t="n"/>
-      <c r="ACC11" s="89" t="n"/>
-      <c r="ACD11" s="89" t="n"/>
-      <c r="ACE11" s="89" t="n"/>
-      <c r="ACF11" s="89" t="n"/>
-      <c r="ACG11" s="89" t="n"/>
-      <c r="ACH11" s="89" t="n"/>
-      <c r="ACI11" s="89" t="n"/>
-      <c r="ACJ11" s="89" t="n"/>
-      <c r="ACK11" s="89" t="n"/>
-      <c r="ACL11" s="89" t="n"/>
-      <c r="ACM11" s="91" t="n"/>
-      <c r="ACN11" s="92" t="n"/>
-      <c r="ACO11" s="92" t="n"/>
-      <c r="ACP11" s="92" t="n"/>
-      <c r="ACQ11" s="92" t="n"/>
-      <c r="ACR11" s="93" t="n"/>
-      <c r="ACS11" s="91" t="n"/>
-      <c r="ACT11" s="92" t="n"/>
-      <c r="ACU11" s="92" t="n"/>
-      <c r="ACV11" s="92" t="n"/>
-      <c r="ACW11" s="92" t="n"/>
-      <c r="ACX11" s="93" t="n"/>
-      <c r="ACY11" s="90" t="n"/>
-      <c r="ACZ11" s="90" t="n"/>
-      <c r="ADA11" s="90" t="n"/>
-      <c r="ADB11" s="90" t="n"/>
+      <c r="XV11" s="107" t="n"/>
+      <c r="XW11" s="107" t="n"/>
+      <c r="XX11" s="107" t="n"/>
+      <c r="XY11" s="105" t="n"/>
+      <c r="XZ11" s="105" t="n"/>
+      <c r="YA11" s="105" t="n"/>
+      <c r="YB11" s="105" t="n"/>
+      <c r="YC11" s="105" t="n"/>
+      <c r="YD11" s="105" t="n"/>
+      <c r="YE11" s="105" t="n"/>
+      <c r="YF11" s="105" t="n"/>
+      <c r="YG11" s="105" t="n"/>
+      <c r="YH11" s="105" t="n"/>
+      <c r="YI11" s="105" t="n"/>
+      <c r="YJ11" s="105" t="n"/>
+      <c r="YK11" s="105" t="n"/>
+      <c r="YL11" s="105" t="n"/>
+      <c r="YM11" s="82" t="n"/>
+      <c r="YN11" s="82" t="n"/>
+      <c r="YO11" s="82" t="n"/>
+      <c r="YP11" s="82" t="n"/>
+      <c r="YQ11" s="82" t="n"/>
+      <c r="YR11" s="82" t="n"/>
+      <c r="YS11" s="82" t="n"/>
+      <c r="YT11" s="82" t="n"/>
+      <c r="YU11" s="82" t="n"/>
+      <c r="YV11" s="82" t="n"/>
+      <c r="YW11" s="82" t="n"/>
+      <c r="YX11" s="82" t="n"/>
+      <c r="YY11" s="82" t="n"/>
+      <c r="YZ11" s="82" t="n"/>
+      <c r="ZA11" s="82" t="n"/>
+      <c r="ZB11" s="82" t="n"/>
+      <c r="ZC11" s="82" t="n"/>
+      <c r="ZD11" s="82" t="n"/>
+      <c r="ZE11" s="82" t="n"/>
+      <c r="ZF11" s="82" t="n"/>
+      <c r="ZG11" s="82" t="n"/>
+      <c r="ZH11" s="83" t="n"/>
+      <c r="ZI11" s="83" t="n"/>
+      <c r="ZJ11" s="83" t="n"/>
+      <c r="ZK11" s="83" t="n"/>
+      <c r="ZL11" s="83" t="n"/>
+      <c r="ZM11" s="83" t="n"/>
+      <c r="ZN11" s="83" t="n"/>
+      <c r="ZO11" s="83" t="n"/>
+      <c r="ZP11" s="83" t="n"/>
+      <c r="ZQ11" s="83" t="n"/>
+      <c r="ZR11" s="83" t="n"/>
+      <c r="ZS11" s="83" t="n"/>
+      <c r="ZT11" s="83" t="n"/>
+      <c r="ZU11" s="83" t="n"/>
+      <c r="ZV11" s="83" t="n"/>
+      <c r="ZW11" s="83" t="n"/>
+      <c r="ZX11" s="83" t="n"/>
+      <c r="ZY11" s="83" t="n"/>
+      <c r="ZZ11" s="83" t="n"/>
+      <c r="AAA11" s="83" t="n"/>
+      <c r="AAB11" s="84" t="n"/>
+      <c r="AAC11" s="84" t="n"/>
+      <c r="AAD11" s="84" t="n"/>
+      <c r="AAE11" s="84" t="n"/>
+      <c r="AAF11" s="84" t="n"/>
+      <c r="AAG11" s="84" t="n"/>
+      <c r="AAH11" s="84" t="n"/>
+      <c r="AAI11" s="84" t="n"/>
+      <c r="AAJ11" s="84" t="n"/>
+      <c r="AAK11" s="84" t="n"/>
+      <c r="AAL11" s="84" t="n"/>
+      <c r="AAM11" s="84" t="n"/>
+      <c r="AAN11" s="84" t="n"/>
+      <c r="AAO11" s="84" t="n"/>
+      <c r="AAP11" s="84" t="n"/>
+      <c r="AAQ11" s="84" t="n"/>
+      <c r="AAR11" s="84" t="n"/>
+      <c r="AAS11" s="84" t="n"/>
+      <c r="AAT11" s="84" t="n"/>
+      <c r="AAU11" s="84" t="n"/>
+      <c r="AAV11" s="84" t="n"/>
+      <c r="AAW11" s="84" t="n"/>
+      <c r="AAX11" s="84" t="n"/>
+      <c r="AAY11" s="84" t="n"/>
+      <c r="AAZ11" s="84" t="n"/>
+      <c r="ABA11" s="84" t="n"/>
+      <c r="ABB11" s="84" t="n"/>
+      <c r="ABC11" s="84" t="n"/>
+      <c r="ABD11" s="84" t="n"/>
+      <c r="ABE11" s="84" t="n"/>
+      <c r="ABF11" s="84" t="n"/>
+      <c r="ABG11" s="84" t="n"/>
+      <c r="ABH11" s="84" t="n"/>
+      <c r="ABI11" s="84" t="n"/>
+      <c r="ABJ11" s="84" t="n"/>
+      <c r="ABK11" s="84" t="n"/>
+      <c r="ABL11" s="84" t="n"/>
+      <c r="ABM11" s="84" t="n"/>
+      <c r="ABN11" s="84" t="n"/>
+      <c r="ABO11" s="84" t="n"/>
+      <c r="ABP11" s="84" t="n"/>
+      <c r="ABQ11" s="84" t="n"/>
+      <c r="ABR11" s="84" t="n"/>
+      <c r="ABS11" s="84" t="n"/>
+      <c r="ABT11" s="84" t="n"/>
+      <c r="ABU11" s="84" t="n"/>
+      <c r="ABV11" s="84" t="n"/>
+      <c r="ABW11" s="84" t="n"/>
+      <c r="ABX11" s="84" t="n"/>
+      <c r="ABY11" s="84" t="n"/>
+      <c r="ABZ11" s="84" t="n"/>
+      <c r="ACA11" s="84" t="n"/>
+      <c r="ACB11" s="84" t="n"/>
+      <c r="ACC11" s="84" t="n"/>
+      <c r="ACD11" s="84" t="n"/>
+      <c r="ACE11" s="84" t="n"/>
+      <c r="ACF11" s="84" t="n"/>
+      <c r="ACG11" s="84" t="n"/>
+      <c r="ACH11" s="84" t="n"/>
+      <c r="ACI11" s="84" t="n"/>
+      <c r="ACJ11" s="84" t="n"/>
+      <c r="ACK11" s="84" t="n"/>
+      <c r="ACL11" s="84" t="n"/>
+      <c r="ACM11" s="86" t="n"/>
+      <c r="ACN11" s="87" t="n"/>
+      <c r="ACO11" s="87" t="n"/>
+      <c r="ACP11" s="87" t="n"/>
+      <c r="ACQ11" s="87" t="n"/>
+      <c r="ACR11" s="88" t="n"/>
+      <c r="ACS11" s="86" t="n"/>
+      <c r="ACT11" s="87" t="n"/>
+      <c r="ACU11" s="87" t="n"/>
+      <c r="ACV11" s="87" t="n"/>
+      <c r="ACW11" s="87" t="n"/>
+      <c r="ACX11" s="88" t="n"/>
+      <c r="ACY11" s="85" t="n"/>
+      <c r="ACZ11" s="85" t="n"/>
+      <c r="ADA11" s="85" t="n"/>
+      <c r="ADB11" s="85" t="n"/>
       <c r="ADC11" s="31" t="n"/>
       <c r="ADD11" s="31" t="n"/>
       <c r="ADE11" s="11" t="n"/>
@@ -55364,7 +55350,7 @@
       <c r="AJQ11" s="11" t="n"/>
       <c r="AJR11" s="11" t="n"/>
       <c r="AJS11" s="11" t="n"/>
-      <c r="AJT11" s="108" t="n"/>
+      <c r="AJT11" s="106" t="n"/>
       <c r="AJU11" s="11" t="n"/>
       <c r="AJV11" s="11" t="n"/>
       <c r="AJW11" s="11" t="n"/>
@@ -55380,74 +55366,74 @@
       <c r="AKG11" s="31" t="n"/>
       <c r="AKH11" s="31" t="n"/>
       <c r="AKI11" s="31" t="n"/>
-      <c r="AKJ11" s="94" t="n"/>
-      <c r="AKK11" s="99" t="n"/>
-      <c r="AKL11" s="100" t="n"/>
-      <c r="AKM11" s="100" t="n"/>
-      <c r="AKN11" s="100" t="n"/>
-      <c r="AKO11" s="101" t="n"/>
-      <c r="AKP11" s="95" t="n"/>
-      <c r="AKQ11" s="109" t="n"/>
-      <c r="AKR11" s="109" t="n"/>
-      <c r="AKS11" s="109" t="n"/>
-      <c r="AKT11" s="109" t="n"/>
-      <c r="AKU11" s="85" t="n"/>
-      <c r="AKV11" s="85" t="n"/>
-      <c r="AKW11" s="85" t="n"/>
-      <c r="AKX11" s="85" t="n"/>
-      <c r="AKY11" s="97" t="n"/>
-      <c r="AKZ11" s="98" t="n"/>
-      <c r="ALA11" s="98" t="n"/>
-      <c r="ALB11" s="98" t="n"/>
-      <c r="ALC11" s="98" t="n"/>
-      <c r="ALD11" s="98" t="n"/>
-      <c r="ALE11" s="98" t="n"/>
-      <c r="ALF11" s="96" t="n"/>
-      <c r="ALG11" s="96" t="n"/>
-      <c r="ALH11" s="98" t="n"/>
-      <c r="ALI11" s="96" t="n"/>
-      <c r="ALJ11" s="96" t="n"/>
-      <c r="ALK11" s="96" t="n"/>
-      <c r="ALL11" s="96" t="n"/>
-      <c r="ALM11" s="96" t="n"/>
-      <c r="ALN11" s="96" t="n"/>
-      <c r="ALO11" s="96" t="n"/>
-      <c r="ALP11" s="96" t="n"/>
-      <c r="ALQ11" s="96" t="n"/>
-      <c r="ALR11" s="96" t="n"/>
-      <c r="ALS11" s="96" t="n"/>
-      <c r="ALT11" s="96" t="n"/>
-      <c r="ALU11" s="96" t="n"/>
-      <c r="ALV11" s="96" t="n"/>
-      <c r="ALW11" s="96" t="n"/>
-      <c r="ALX11" s="96" t="n"/>
-      <c r="ALY11" s="96" t="n"/>
-      <c r="ALZ11" s="96" t="n"/>
-      <c r="AMA11" s="96" t="n"/>
-      <c r="AMB11" s="96" t="n"/>
-      <c r="AMC11" s="96" t="n"/>
-      <c r="AMD11" s="96" t="n"/>
-      <c r="AME11" s="96" t="n"/>
-      <c r="AMF11" s="96" t="n"/>
-      <c r="AMG11" s="96" t="n"/>
-      <c r="AMH11" s="96" t="n"/>
-      <c r="AMI11" s="96" t="n"/>
-      <c r="AMJ11" s="96" t="n"/>
-      <c r="AMK11" s="96" t="n"/>
-      <c r="AML11" s="96" t="n"/>
-      <c r="AMM11" s="96" t="n"/>
-      <c r="AMN11" s="96" t="n"/>
-      <c r="AMO11" s="96" t="n"/>
-      <c r="AMP11" s="96" t="n"/>
-      <c r="AMQ11" s="96" t="n"/>
-      <c r="AMR11" s="96" t="n"/>
-      <c r="AMS11" s="96" t="n"/>
-      <c r="AMT11" s="96" t="n"/>
-      <c r="AMU11" s="96" t="n"/>
-      <c r="AMV11" s="96" t="n"/>
-      <c r="AMW11" s="96" t="n"/>
-      <c r="AMX11" s="96" t="n"/>
-      <c r="AMY11" s="96" t="n"/>
+      <c r="AKJ11" s="89" t="n"/>
+      <c r="AKK11" s="94" t="n"/>
+      <c r="AKL11" s="95" t="n"/>
+      <c r="AKM11" s="95" t="n"/>
+      <c r="AKN11" s="95" t="n"/>
+      <c r="AKO11" s="96" t="n"/>
+      <c r="AKP11" s="90" t="n"/>
+      <c r="AKQ11" s="107" t="n"/>
+      <c r="AKR11" s="107" t="n"/>
+      <c r="AKS11" s="107" t="n"/>
+      <c r="AKT11" s="107" t="n"/>
+      <c r="AKU11" s="80" t="n"/>
+      <c r="AKV11" s="80" t="n"/>
+      <c r="AKW11" s="80" t="n"/>
+      <c r="AKX11" s="80" t="n"/>
+      <c r="AKY11" s="92" t="n"/>
+      <c r="AKZ11" s="93" t="n"/>
+      <c r="ALA11" s="93" t="n"/>
+      <c r="ALB11" s="93" t="n"/>
+      <c r="ALC11" s="93" t="n"/>
+      <c r="ALD11" s="93" t="n"/>
+      <c r="ALE11" s="93" t="n"/>
+      <c r="ALF11" s="91" t="n"/>
+      <c r="ALG11" s="91" t="n"/>
+      <c r="ALH11" s="93" t="n"/>
+      <c r="ALI11" s="91" t="n"/>
+      <c r="ALJ11" s="91" t="n"/>
+      <c r="ALK11" s="91" t="n"/>
+      <c r="ALL11" s="91" t="n"/>
+      <c r="ALM11" s="91" t="n"/>
+      <c r="ALN11" s="91" t="n"/>
+      <c r="ALO11" s="91" t="n"/>
+      <c r="ALP11" s="91" t="n"/>
+      <c r="ALQ11" s="91" t="n"/>
+      <c r="ALR11" s="91" t="n"/>
+      <c r="ALS11" s="91" t="n"/>
+      <c r="ALT11" s="91" t="n"/>
+      <c r="ALU11" s="91" t="n"/>
+      <c r="ALV11" s="91" t="n"/>
+      <c r="ALW11" s="91" t="n"/>
+      <c r="ALX11" s="91" t="n"/>
+      <c r="ALY11" s="91" t="n"/>
+      <c r="ALZ11" s="91" t="n"/>
+      <c r="AMA11" s="91" t="n"/>
+      <c r="AMB11" s="91" t="n"/>
+      <c r="AMC11" s="91" t="n"/>
+      <c r="AMD11" s="91" t="n"/>
+      <c r="AME11" s="91" t="n"/>
+      <c r="AMF11" s="91" t="n"/>
+      <c r="AMG11" s="91" t="n"/>
+      <c r="AMH11" s="91" t="n"/>
+      <c r="AMI11" s="91" t="n"/>
+      <c r="AMJ11" s="91" t="n"/>
+      <c r="AMK11" s="91" t="n"/>
+      <c r="AML11" s="91" t="n"/>
+      <c r="AMM11" s="91" t="n"/>
+      <c r="AMN11" s="91" t="n"/>
+      <c r="AMO11" s="91" t="n"/>
+      <c r="AMP11" s="91" t="n"/>
+      <c r="AMQ11" s="91" t="n"/>
+      <c r="AMR11" s="91" t="n"/>
+      <c r="AMS11" s="91" t="n"/>
+      <c r="AMT11" s="91" t="n"/>
+      <c r="AMU11" s="91" t="n"/>
+      <c r="AMV11" s="91" t="n"/>
+      <c r="AMW11" s="91" t="n"/>
+      <c r="AMX11" s="91" t="n"/>
+      <c r="AMY11" s="91" t="n"/>
       <c r="AON11" s="20" t="inlineStr">
         <is>
           <t>Induction</t>
@@ -55606,7 +55592,7 @@
           <t>On</t>
         </is>
       </c>
-      <c r="APT11" s="102" t="inlineStr">
+      <c r="APT11" s="97" t="inlineStr">
         <is>
           <t>WOH Training</t>
         </is>
@@ -56017,262 +56003,259 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="15.6" customHeight="1">
-      <c r="A12" s="77" t="inlineStr">
-        <is>
-          <t>Site Manager</t>
-        </is>
-      </c>
-      <c r="B12" s="78" t="inlineStr">
-        <is>
-          <t>Miguel Venegas</t>
-        </is>
-      </c>
-      <c r="C12" s="74" t="inlineStr">
-        <is>
-          <t>TP0352</t>
-        </is>
-      </c>
-      <c r="ARB12" s="84" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Fuel Attendants</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Aloekoe Figaro</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TP0904</t>
+        </is>
+      </c>
+      <c r="ARS12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARC12" s="84" t="inlineStr">
+      <c r="ART12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARD12" s="84" t="inlineStr">
+      <c r="ARU12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARE12" s="84" t="inlineStr">
+      <c r="ARV12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARF12" s="84" t="inlineStr">
+      <c r="ARW12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARG12" s="84" t="inlineStr">
+      <c r="ARX12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARH12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARI12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARJ12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARK12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARL12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARM12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARN12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARO12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARP12" s="84" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARZ12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASA12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASB12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASC12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASD12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASE12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASF12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASG12" s="103" t="inlineStr">
-        <is>
-          <t>ON</t>
+      <c r="ARY12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARZ12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASA12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASB12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASC12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASD12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASE12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASF12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASG12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASH12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASI12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASJ12" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15.6" customHeight="1">
-      <c r="A13" s="77" t="inlineStr">
-        <is>
-          <t>Data Analyst</t>
-        </is>
-      </c>
-      <c r="B13" s="78" t="inlineStr">
-        <is>
-          <t>Jose Gomez</t>
-        </is>
-      </c>
-      <c r="C13" s="74" t="inlineStr">
-        <is>
-          <t>TP0039</t>
-        </is>
-      </c>
-      <c r="ARB13" s="84" t="n"/>
-      <c r="ARC13" s="84" t="n"/>
-      <c r="ARD13" s="84" t="n"/>
-      <c r="ARE13" s="84" t="n"/>
-      <c r="ARF13" s="84" t="n"/>
-      <c r="ARG13" s="84" t="n"/>
-      <c r="ARH13" s="84" t="n"/>
-      <c r="ARI13" s="84" t="n"/>
-      <c r="ARJ13" s="84" t="n"/>
-      <c r="ARK13" s="84" t="n"/>
-      <c r="ARL13" s="84" t="n"/>
-      <c r="ARM13" s="84" t="n"/>
-      <c r="ARN13" s="84" t="n"/>
-      <c r="ARO13" s="84" t="n"/>
-      <c r="ARP13" s="84" t="n"/>
-      <c r="ARZ13" s="103" t="n"/>
-      <c r="ASA13" s="103" t="n"/>
-      <c r="ASB13" s="103" t="n"/>
-      <c r="ASC13" s="103" t="n"/>
-      <c r="ASD13" s="103" t="n"/>
-      <c r="ASE13" s="103" t="n"/>
-      <c r="ASF13" s="103" t="n"/>
-      <c r="ASG13" s="103" t="n"/>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Fuel Attendants</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Juan Hernandez</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>TP1234</t>
+        </is>
+      </c>
+      <c r="ARP13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARQ13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARR13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARS13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ART13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARU13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARV13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ARW13" s="109" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vincent Rolong </t>
+          <t>Rosa Merlano</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>12345678</t>
-        </is>
-      </c>
-      <c r="ARG14" s="110" t="inlineStr">
+          <t>TP0903</t>
+        </is>
+      </c>
+      <c r="ARP14" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARH14" s="110" t="inlineStr">
+      <c r="ARQ14" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARI14" s="110" t="inlineStr">
+      <c r="ARR14" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARJ14" s="110" t="inlineStr">
+      <c r="ARS14" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARK14" s="110" t="inlineStr">
+      <c r="ART14" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARL14" s="110" t="inlineStr">
+      <c r="ARU14" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARN14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARO14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARP14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARQ14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARR14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARS14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ART14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARU14" s="111" t="inlineStr">
-        <is>
-          <t>ON NS</t>
+      <c r="ARV14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARW14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARX14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARY14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARZ14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASA14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASB14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASC14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASD14" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>